<commit_message>
xpath added for BUS
</commit_message>
<xml_diff>
--- a/Problem1.xlsx
+++ b/Problem1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myworkspace\SeleniumAssignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,6 +82,7 @@
   </si>
   <si>
     <t>//a[contains(@class, 'nav-list-item u-uppercase u-ib  u-nostyle-link')]
+//a[text()='BUSES']
 //nav::span[3]</t>
   </si>
 </sst>
@@ -435,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>